<commit_message>
xong he so bg
</commit_message>
<xml_diff>
--- a/uploads/excel.xlsx
+++ b/uploads/excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Lap Trinh\NodeJs\BocThamVongTron\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56F6F6D-BC00-424E-AA15-B118B5DA5E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F90566E-DCA7-42EF-8BEA-E82F717B81C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{24C2CB95-7022-49C4-B371-12CE8A8138D6}"/>
   </bookViews>
@@ -77,9 +77,6 @@
 (Chú ý có bao nhiêu vđv thì để bấy nhiêu dòng, xóa các dòng còn thừa)</t>
   </si>
   <si>
-    <t>Lê Quang Liêm</t>
-  </si>
-  <si>
     <t>Phùng Thị Tuyết Lan</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>HCM</t>
+  </si>
+  <si>
+    <t>Co Ca</t>
   </si>
 </sst>
 </file>
@@ -495,7 +495,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,7 +569,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>10</v>
@@ -580,10 +580,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -591,7 +591,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
@@ -602,7 +602,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
xong he so doi khang truc tiep
</commit_message>
<xml_diff>
--- a/uploads/excel.xlsx
+++ b/uploads/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F90566E-DCA7-42EF-8BEA-E82F717B81C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950FB125-9446-4313-BF02-4C90341F6530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{24C2CB95-7022-49C4-B371-12CE8A8138D6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>STT</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>Chim Sẻ Đi Nắng</t>
-  </si>
-  <si>
-    <t>HCM</t>
   </si>
   <si>
     <t>Co Ca</t>
@@ -495,7 +492,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -580,11 +577,9 @@
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="5">

</xml_diff>

<commit_message>
lan dau up server
</commit_message>
<xml_diff>
--- a/uploads/excel.xlsx
+++ b/uploads/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950FB125-9446-4313-BF02-4C90341F6530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5797ADF1-50E1-4864-93DD-8B839505BBB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{24C2CB95-7022-49C4-B371-12CE8A8138D6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>STT</t>
   </si>
@@ -77,16 +77,16 @@
 (Chú ý có bao nhiêu vđv thì để bấy nhiêu dòng, xóa các dòng còn thừa)</t>
   </si>
   <si>
+    <t>Lê Quang Liêm</t>
+  </si>
+  <si>
     <t>Phùng Thị Tuyết Lan</t>
   </si>
   <si>
     <t>Lê Tuấn Minh</t>
   </si>
   <si>
-    <t>Chim Sẻ Đi Nắng</t>
-  </si>
-  <si>
-    <t>Co Ca</t>
+    <t>HCM</t>
   </si>
 </sst>
 </file>
@@ -489,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F1B2A19-02D0-409B-ADA0-EF63FDFFA6FD}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,7 +566,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>10</v>
@@ -577,31 +577,25 @@
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
-        <v>7</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>9</v>
-      </c>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11"/>
@@ -629,9 +623,6 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
xong co ban ve dem va chinh sua fix 1 so thu
</commit_message>
<xml_diff>
--- a/uploads/excel.xlsx
+++ b/uploads/excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5797ADF1-50E1-4864-93DD-8B839505BBB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1D97AF-EC21-41E1-A92B-A2F62A18DFBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{24C2CB95-7022-49C4-B371-12CE8A8138D6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>STT</t>
   </si>
@@ -50,13 +50,7 @@
     <t>BẢNG MẪU DANH SÁCH VĐV CẦN BỐC THĂM VÒNG TRÒN</t>
   </si>
   <si>
-    <t>Thầy Toàn Cờ Vua</t>
-  </si>
-  <si>
     <t>Quân Đội</t>
-  </si>
-  <si>
-    <t>Lê Trọng Đề Toàn</t>
   </si>
   <si>
     <t>Thanh Hóa</t>
@@ -86,7 +80,19 @@
     <t>Lê Tuấn Minh</t>
   </si>
   <si>
+    <t>Chim Sẻ Đi Nắng</t>
+  </si>
+  <si>
     <t>HCM</t>
+  </si>
+  <si>
+    <t>Thầy Toàn Cờ Vua 1</t>
+  </si>
+  <si>
+    <t>Lê Trọng Đề Toàn 2</t>
+  </si>
+  <si>
+    <t>hh</t>
   </si>
 </sst>
 </file>
@@ -489,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F1B2A19-02D0-409B-ADA0-EF63FDFFA6FD}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,7 +517,7 @@
     </row>
     <row r="2" spans="1:7" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -533,10 +539,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -544,10 +550,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -555,10 +561,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -566,10 +572,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -577,10 +583,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -588,20 +594,44 @@
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>9</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13"/>
@@ -614,15 +644,6 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>